<commit_message>
worker recording validation and exception path test cases
</commit_message>
<xml_diff>
--- a/soberano/test_cases/worker_record_test_cases.xlsx
+++ b/soberano/test_cases/worker_record_test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="42">
   <si>
     <t xml:space="preserve">TC Number</t>
   </si>
@@ -107,6 +107,45 @@
   </si>
   <si>
     <t xml:space="preserve">Plaza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username isn’t valid email address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manager@soberano.syscoop.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmed password empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First name empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Last name empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Province empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Municipality empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password don’t match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Worker must be assigned to a responsibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not enough rights</t>
   </si>
 </sst>
 </file>
@@ -116,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -144,6 +183,18 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Monospace"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -188,12 +239,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -206,6 +265,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF2A00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -214,16 +333,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ31"/>
+  <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="15.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.85"/>
@@ -359,56 +480,617 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="B8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="B10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="B11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>1234</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S11" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>12345</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>55555555</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>54321</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>-81</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -498,6 +1180,351 @@
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>30</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worker modification test case 3
</commit_message>
<xml_diff>
--- a/soberano/test_cases/worker_record_test_cases.xlsx
+++ b/soberano/test_cases/worker_record_test_cases.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="192">
   <si>
     <t xml:space="preserve">TC Number</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test constrained (for input validation) form components</t>
   </si>
   <si>
     <t xml:space="preserve">Username empty</t>
@@ -731,10 +734,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ100"/>
+  <dimension ref="A1:AMJ101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -822,72 +825,21 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>12345</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>12345</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>55555555</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>54321</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="R2" s="3" t="n">
-        <v>21</v>
-      </c>
-      <c r="S2" s="3" t="n">
-        <v>-81</v>
-      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>12345</v>
@@ -896,40 +848,37 @@
         <v>12345</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I3" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L3" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R3" s="3" t="n">
         <v>21</v>
@@ -940,52 +889,52 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>32</v>
+      <c r="D4" s="2" t="n">
+        <v>12345</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>12345</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I4" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R4" s="3" t="n">
         <v>21</v>
@@ -996,52 +945,49 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="2" t="n">
+      <c r="E5" s="2" t="n">
         <v>12345</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L5" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R5" s="3" t="n">
         <v>21</v>
@@ -1052,52 +998,49 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>12345</v>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>12345</v>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L6" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R6" s="3" t="n">
         <v>21</v>
@@ -1108,13 +1051,13 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>12345</v>
@@ -1122,38 +1065,35 @@
       <c r="E7" s="2" t="n">
         <v>12345</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I7" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L7" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R7" s="3" t="n">
         <v>21</v>
@@ -1164,13 +1104,13 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>12345</v>
@@ -1179,37 +1119,34 @@
         <v>12345</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I8" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L8" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="P8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R8" s="3" t="n">
         <v>21</v>
@@ -1220,13 +1157,13 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>12345</v>
@@ -1235,37 +1172,34 @@
         <v>12345</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L9" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O9" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="P9" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="Q9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R9" s="3" t="n">
         <v>21</v>
@@ -1276,13 +1210,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>12345</v>
@@ -1291,37 +1225,34 @@
         <v>12345</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I10" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L10" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>27</v>
+        <v>27</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="R10" s="3" t="n">
         <v>21</v>
@@ -1332,54 +1263,48 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>12345</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>1234</v>
+        <v>12345</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="I11" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L11" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R11" s="3" t="n">
@@ -1391,49 +1316,52 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>12345</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>12345</v>
+        <v>1234</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I12" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L12" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R12" s="3" t="n">
         <v>21</v>
@@ -1444,13 +1372,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>12345</v>
@@ -1458,41 +1386,32 @@
       <c r="E13" s="2" t="n">
         <v>12345</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I13" s="1" t="n">
         <v>55555555</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R13" s="3" t="n">
         <v>21</v>
@@ -1503,13 +1422,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>12345</v>
@@ -1518,37 +1437,37 @@
         <v>12345</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>20</v>
+      <c r="I14" s="1" t="n">
+        <v>55555555</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L14" s="1" t="n">
         <v>54321</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R14" s="3" t="n">
         <v>21</v>
@@ -1559,409 +1478,385 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>45</v>
+      <c r="C15" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>12345</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>12345</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>50155555</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>48</v>
+        <v>24</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <v>54321</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="R15" s="3" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="S15" s="3" t="n">
-        <v>1</v>
+        <v>-81</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>50155555</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>50255555</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="R16" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S16" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>50255555</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q17" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <v>50355555</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P17" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q17" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="R17" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S17" s="3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>50355555</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>50455555</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="R18" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S18" s="3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>50455555</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>50555555</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q19" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="R19" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S19" s="3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>50555555</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>50655555</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="R20" s="3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S20" s="3" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I21" s="1" t="n">
         <v>50655555</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K21" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="R21" s="3" t="n">
         <v>6</v>
@@ -1972,232 +1867,220 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>50755555</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>20</v>
+        <v>50655555</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="R22" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S22" s="3" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>50755555</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q23" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <v>50855555</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="R23" s="3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="S23" s="3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>50855555</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q24" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <v>50955555</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="L24" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M24" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P24" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="R24" s="3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="S24" s="3" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="I25" s="1" t="n">
         <v>50955555</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K25" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M25" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="R25" s="3" t="n">
         <v>9</v>
@@ -2208,114 +2091,108 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>51055555</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>20</v>
+        <v>50955555</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="R26" s="3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="S26" s="3" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I27" s="1" t="n">
         <v>51055555</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K27" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="R27" s="3" t="n">
         <v>10</v>
@@ -2326,55 +2203,52 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>144</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I28" s="1" t="n">
         <v>51055555</v>
       </c>
-      <c r="J28" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K28" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="R28" s="3" t="n">
         <v>10</v>
@@ -2385,55 +2259,52 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I29" s="1" t="n">
         <v>51055555</v>
       </c>
-      <c r="J29" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K29" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="R29" s="3" t="n">
         <v>10</v>
@@ -2444,232 +2315,220 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>146</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>51155555</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>20</v>
+        <v>51055555</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="R30" s="3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S30" s="3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>51155555</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q31" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="I31" s="1" t="n">
-        <v>51255555</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="R31" s="3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S31" s="3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>51255555</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q32" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I32" s="1" t="n">
-        <v>51355555</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="L32" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="R32" s="3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S32" s="3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="I33" s="1" t="n">
         <v>51355555</v>
       </c>
-      <c r="J33" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K33" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="R33" s="3" t="n">
         <v>13</v>
@@ -2680,15 +2539,63 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>178</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>51355555</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="R34" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="S34" s="3" t="n">
+        <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>179</v>
@@ -2696,7 +2603,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>180</v>
@@ -2704,7 +2611,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>181</v>
@@ -2712,7 +2619,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>182</v>
@@ -2720,7 +2627,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>183</v>
@@ -2728,7 +2635,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>184</v>
@@ -2736,7 +2643,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>185</v>
@@ -2744,7 +2651,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>186</v>
@@ -2752,7 +2659,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>187</v>
@@ -2760,7 +2667,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>188</v>
@@ -2768,7 +2675,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>189</v>
@@ -2776,7 +2683,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>190</v>
@@ -2784,271 +2691,279 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="n">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="n">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="n">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="n">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="n">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="n">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="n">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="1" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="n">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="n">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="n">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1" t="n">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="1" t="n">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="1" t="n">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="1" t="n">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="1" t="n">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="n">
         <v>99</v>
       </c>
     </row>

</xml_diff>